<commit_message>
Modify the UI elements
Modify the UI elements
</commit_message>
<xml_diff>
--- a/Assets/testResult.xlsx
+++ b/Assets/testResult.xlsx
@@ -644,7 +644,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="56">
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="43" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="1" applyProtection="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -790,6 +790,10 @@
     <xf numFmtId="0" applyNumberFormat="1" fontId="19" applyFont="1" fillId="32" applyFill="1" borderId="0" applyBorder="1" xfId="48" applyProtection="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
@@ -1326,7 +1330,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
@@ -1335,485 +1339,577 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="6"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="51" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="51" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="51" t="s">
+      <c r="B1" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="55" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="E1" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="51" t="s">
+      <c r="F1" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="51" t="s">
+      <c r="G1" s="55" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="51">
-        <v>1</v>
-      </c>
-      <c r="B2" s="51">
+      <c r="A2" s="55">
+        <v>1</v>
+      </c>
+      <c r="B2" s="55">
         <v>0.100000001490116</v>
       </c>
-      <c r="C2" s="51">
+      <c r="C2" s="55">
         <v>50</v>
       </c>
-      <c r="D2" s="51">
-        <v>2</v>
-      </c>
-      <c r="E2" s="51">
-        <v>2</v>
-      </c>
-      <c r="F2" s="51" t="s">
+      <c r="D2" s="55">
+        <v>2</v>
+      </c>
+      <c r="E2" s="55">
+        <v>2</v>
+      </c>
+      <c r="F2" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="51">
+      <c r="G2" s="55">
         <v>1</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="51">
-        <v>2</v>
-      </c>
-      <c r="B3" s="51">
+      <c r="A3" s="55">
+        <v>2</v>
+      </c>
+      <c r="B3" s="55">
         <v>0.100000001490116</v>
       </c>
-      <c r="C3" s="51">
+      <c r="C3" s="55">
         <v>50</v>
       </c>
-      <c r="D3" s="51">
-        <v>2</v>
-      </c>
-      <c r="E3" s="51">
+      <c r="D3" s="55">
+        <v>2</v>
+      </c>
+      <c r="E3" s="55">
         <v>2.2999997138977</v>
       </c>
-      <c r="F3" s="51" t="s">
+      <c r="F3" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="51">
+      <c r="G3" s="55">
         <v>1</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="51">
+      <c r="A4" s="55">
         <v>3</v>
       </c>
-      <c r="B4" s="51">
+      <c r="B4" s="55">
         <v>0.100000001490116</v>
       </c>
-      <c r="C4" s="51">
+      <c r="C4" s="55">
         <v>50</v>
       </c>
-      <c r="D4" s="51">
-        <v>2</v>
-      </c>
-      <c r="E4" s="51">
+      <c r="D4" s="55">
+        <v>2</v>
+      </c>
+      <c r="E4" s="55">
         <v>2.2999997138977</v>
       </c>
-      <c r="F4" s="51" t="s">
+      <c r="F4" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="51">
+      <c r="G4" s="55">
         <v>1</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="51">
+      <c r="A5" s="55">
         <v>4</v>
       </c>
-      <c r="B5" s="51">
+      <c r="B5" s="55">
         <v>0.100000001490116</v>
       </c>
-      <c r="C5" s="51">
+      <c r="C5" s="55">
         <v>50</v>
       </c>
-      <c r="D5" s="51">
-        <v>2</v>
-      </c>
-      <c r="E5" s="51">
+      <c r="D5" s="55">
+        <v>2</v>
+      </c>
+      <c r="E5" s="55">
         <v>2.2999997138977</v>
       </c>
-      <c r="F5" s="51" t="s">
+      <c r="F5" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="51">
+      <c r="G5" s="55">
         <v>1</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="51">
+      <c r="A6" s="55">
         <v>5</v>
       </c>
-      <c r="B6" s="51">
+      <c r="B6" s="55">
         <v>0.100000001490116</v>
       </c>
-      <c r="C6" s="51">
+      <c r="C6" s="55">
         <v>50</v>
       </c>
-      <c r="D6" s="51">
-        <v>2</v>
-      </c>
-      <c r="E6" s="51">
+      <c r="D6" s="55">
+        <v>2</v>
+      </c>
+      <c r="E6" s="55">
         <v>2.59999942779541</v>
       </c>
-      <c r="F6" s="51" t="s">
+      <c r="F6" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="51">
+      <c r="G6" s="55">
         <v>1</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="51">
+      <c r="A7" s="55">
         <v>6</v>
       </c>
-      <c r="B7" s="51">
+      <c r="B7" s="55">
         <v>0.100000001490116</v>
       </c>
-      <c r="C7" s="51">
+      <c r="C7" s="55">
         <v>50</v>
       </c>
-      <c r="D7" s="51">
-        <v>2</v>
-      </c>
-      <c r="E7" s="51">
-        <v>2</v>
-      </c>
-      <c r="F7" s="51" t="s">
+      <c r="D7" s="55">
+        <v>2</v>
+      </c>
+      <c r="E7" s="55">
+        <v>2</v>
+      </c>
+      <c r="F7" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="51">
+      <c r="G7" s="55">
         <v>1</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="51">
+      <c r="A8" s="55">
         <v>7</v>
       </c>
-      <c r="B8" s="51">
+      <c r="B8" s="55">
         <v>0.100000001490116</v>
       </c>
-      <c r="C8" s="51">
+      <c r="C8" s="55">
         <v>50</v>
       </c>
-      <c r="D8" s="51">
-        <v>2</v>
-      </c>
-      <c r="E8" s="51">
-        <v>2</v>
-      </c>
-      <c r="F8" s="51" t="s">
+      <c r="D8" s="55">
+        <v>2</v>
+      </c>
+      <c r="E8" s="55">
+        <v>2</v>
+      </c>
+      <c r="F8" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="51">
+      <c r="G8" s="55">
         <v>1</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="51">
+      <c r="A9" s="55">
         <v>8</v>
       </c>
-      <c r="B9" s="51">
+      <c r="B9" s="55">
         <v>0.100000001490116</v>
       </c>
-      <c r="C9" s="51">
+      <c r="C9" s="55">
         <v>50</v>
       </c>
-      <c r="D9" s="51">
-        <v>2</v>
-      </c>
-      <c r="E9" s="51">
-        <v>2</v>
-      </c>
-      <c r="F9" s="51" t="s">
+      <c r="D9" s="55">
+        <v>2</v>
+      </c>
+      <c r="E9" s="55">
+        <v>2</v>
+      </c>
+      <c r="F9" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="51">
+      <c r="G9" s="55">
         <v>1</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="51">
+      <c r="A10" s="55">
         <v>9</v>
       </c>
-      <c r="B10" s="51">
+      <c r="B10" s="55">
         <v>0.100000001490116</v>
       </c>
-      <c r="C10" s="51">
+      <c r="C10" s="55">
         <v>50</v>
       </c>
-      <c r="D10" s="51">
-        <v>2</v>
-      </c>
-      <c r="E10" s="51">
+      <c r="D10" s="55">
+        <v>2</v>
+      </c>
+      <c r="E10" s="55">
         <v>2.39999961853027</v>
       </c>
-      <c r="F10" s="51" t="s">
+      <c r="F10" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="51">
+      <c r="G10" s="55">
         <v>1</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="51">
+      <c r="A11" s="55">
         <v>10</v>
       </c>
-      <c r="B11" s="51">
+      <c r="B11" s="55">
         <v>0.100000001490116</v>
       </c>
-      <c r="C11" s="51">
+      <c r="C11" s="55">
         <v>50</v>
       </c>
-      <c r="D11" s="51">
-        <v>2</v>
-      </c>
-      <c r="E11" s="51">
+      <c r="D11" s="55">
+        <v>2</v>
+      </c>
+      <c r="E11" s="55">
         <v>2.2999997138977</v>
       </c>
-      <c r="F11" s="51" t="s">
+      <c r="F11" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="51">
+      <c r="G11" s="55">
         <v>1</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="51">
+      <c r="A12" s="55">
         <v>11</v>
       </c>
-      <c r="B12" s="51">
+      <c r="B12" s="55">
         <v>0.100000001490116</v>
       </c>
-      <c r="C12" s="51">
+      <c r="C12" s="55">
         <v>50</v>
       </c>
-      <c r="D12" s="51">
-        <v>2</v>
-      </c>
-      <c r="E12" s="51">
+      <c r="D12" s="55">
+        <v>2</v>
+      </c>
+      <c r="E12" s="55">
         <v>2.79999923706055</v>
       </c>
-      <c r="F12" s="51" t="s">
+      <c r="F12" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="G12" s="51">
+      <c r="G12" s="55">
         <v>1</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="51">
+      <c r="A13" s="55">
         <v>12</v>
       </c>
-      <c r="B13" s="51">
+      <c r="B13" s="55">
         <v>0.100000001490116</v>
       </c>
-      <c r="C13" s="51">
+      <c r="C13" s="55">
         <v>50</v>
       </c>
-      <c r="D13" s="51">
+      <c r="D13" s="55">
         <v>2.57806086540222</v>
       </c>
-      <c r="E13" s="51">
-        <v>2</v>
-      </c>
-      <c r="F13" s="51" t="s">
+      <c r="E13" s="55">
+        <v>2</v>
+      </c>
+      <c r="F13" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="G13" s="51">
+      <c r="G13" s="55">
         <v>1</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="51">
+      <c r="A14" s="55">
         <v>13</v>
       </c>
-      <c r="B14" s="51">
+      <c r="B14" s="55">
         <v>0.100000001490116</v>
       </c>
-      <c r="C14" s="51">
+      <c r="C14" s="55">
         <v>60</v>
       </c>
-      <c r="D14" s="51">
-        <v>2</v>
-      </c>
-      <c r="E14" s="51">
-        <v>2</v>
-      </c>
-      <c r="F14" s="51" t="s">
+      <c r="D14" s="55">
+        <v>2</v>
+      </c>
+      <c r="E14" s="55">
+        <v>2</v>
+      </c>
+      <c r="F14" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="G14" s="51">
+      <c r="G14" s="55">
         <v>1</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="51">
+      <c r="A15" s="55">
         <v>14</v>
       </c>
-      <c r="B15" s="51">
+      <c r="B15" s="55">
         <v>0.100000001490116</v>
       </c>
-      <c r="C15" s="51">
+      <c r="C15" s="55">
         <v>146.781585693359</v>
       </c>
-      <c r="D15" s="51">
-        <v>2</v>
-      </c>
-      <c r="E15" s="51">
-        <v>2</v>
-      </c>
-      <c r="F15" s="51" t="s">
+      <c r="D15" s="55">
+        <v>2</v>
+      </c>
+      <c r="E15" s="55">
+        <v>2</v>
+      </c>
+      <c r="F15" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="G15" s="51">
+      <c r="G15" s="55">
         <v>1</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="51">
+      <c r="A16" s="55">
         <v>15</v>
       </c>
-      <c r="B16" s="51">
+      <c r="B16" s="55">
         <v>0.100000001490116</v>
       </c>
-      <c r="C16" s="51">
+      <c r="C16" s="55">
         <v>146.781585693359</v>
       </c>
-      <c r="D16" s="51">
-        <v>2</v>
-      </c>
-      <c r="E16" s="51">
-        <v>2</v>
-      </c>
-      <c r="F16" s="51" t="s">
+      <c r="D16" s="55">
+        <v>2</v>
+      </c>
+      <c r="E16" s="55">
+        <v>2</v>
+      </c>
+      <c r="F16" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="G16" s="51">
+      <c r="G16" s="55">
         <v>1</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="51">
+      <c r="A17" s="55">
         <v>16</v>
       </c>
-      <c r="B17" s="51">
+      <c r="B17" s="55">
         <v>0.100000001490116</v>
       </c>
-      <c r="C17" s="51">
+      <c r="C17" s="55">
         <v>146.781585693359</v>
       </c>
-      <c r="D17" s="51">
-        <v>2</v>
-      </c>
-      <c r="E17" s="51">
-        <v>2</v>
-      </c>
-      <c r="F17" s="51" t="s">
+      <c r="D17" s="55">
+        <v>2</v>
+      </c>
+      <c r="E17" s="55">
+        <v>2</v>
+      </c>
+      <c r="F17" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="G17" s="51">
+      <c r="G17" s="55">
         <v>1</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="51">
+      <c r="A18" s="55">
         <v>17</v>
       </c>
-      <c r="B18" s="51">
+      <c r="B18" s="55">
         <v>0.413215100765228</v>
       </c>
-      <c r="C18" s="51">
+      <c r="C18" s="55">
         <v>50</v>
       </c>
-      <c r="D18" s="51">
-        <v>2</v>
-      </c>
-      <c r="E18" s="51">
-        <v>2</v>
-      </c>
-      <c r="F18" s="51" t="s">
+      <c r="D18" s="55">
+        <v>2</v>
+      </c>
+      <c r="E18" s="55">
+        <v>2</v>
+      </c>
+      <c r="F18" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="G18" s="51">
+      <c r="G18" s="55">
         <v>1</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="51">
+      <c r="A19" s="55">
         <v>18</v>
       </c>
-      <c r="B19" s="51">
+      <c r="B19" s="55">
         <v>0.10000000149011612</v>
       </c>
-      <c r="C19" s="51">
+      <c r="C19" s="55">
         <v>50</v>
       </c>
-      <c r="D19" s="51">
-        <v>2</v>
-      </c>
-      <c r="E19" s="51">
-        <v>2</v>
-      </c>
-      <c r="F19" s="51" t="s">
+      <c r="D19" s="55">
+        <v>2</v>
+      </c>
+      <c r="E19" s="55">
+        <v>2</v>
+      </c>
+      <c r="F19" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="G19" s="51">
+      <c r="G19" s="55">
         <v>1</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="50">
+      <c r="A20" s="54">
         <v>19</v>
       </c>
-      <c r="B20" s="50">
+      <c r="B20" s="54">
         <v>0.27679422497749329</v>
       </c>
-      <c r="C20" s="50">
+      <c r="C20" s="54">
         <v>50</v>
       </c>
-      <c r="D20" s="50">
-        <v>2</v>
-      </c>
-      <c r="E20" s="50">
-        <v>2</v>
-      </c>
-      <c r="F20" s="50" t="s">
+      <c r="D20" s="54">
+        <v>2</v>
+      </c>
+      <c r="E20" s="54">
+        <v>2</v>
+      </c>
+      <c r="F20" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="G20" s="50">
+      <c r="G20" s="54">
         <v>1</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="49">
+      <c r="A21" s="53">
         <v>20</v>
       </c>
-      <c r="B21" s="49">
+      <c r="B21" s="53">
         <v>0.10000000149011612</v>
       </c>
-      <c r="C21" s="49">
+      <c r="C21" s="53">
         <v>50</v>
       </c>
-      <c r="D21" s="49">
+      <c r="D21" s="53">
         <v>2.9559769630432129</v>
       </c>
-      <c r="E21" s="49">
-        <v>2</v>
-      </c>
-      <c r="F21" s="49" t="s">
+      <c r="E21" s="53">
+        <v>2</v>
+      </c>
+      <c r="F21" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="G21" s="49">
+      <c r="G21" s="53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="52">
+        <v>21</v>
+      </c>
+      <c r="B22" s="52">
+        <v>0.16000001132488251</v>
+      </c>
+      <c r="C22" s="52">
+        <v>100</v>
+      </c>
+      <c r="D22" s="52">
+        <v>2</v>
+      </c>
+      <c r="E22" s="52">
+        <v>2</v>
+      </c>
+      <c r="F22" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" s="52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="51">
+        <v>22</v>
+      </c>
+      <c r="B23" s="51">
+        <v>0.14999999105930328</v>
+      </c>
+      <c r="C23" s="51">
+        <v>100</v>
+      </c>
+      <c r="D23" s="51">
+        <v>2</v>
+      </c>
+      <c r="E23" s="51">
+        <v>2</v>
+      </c>
+      <c r="F23" s="51" t="s">
+        <v>8</v>
+      </c>
+      <c r="G23" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="50">
+        <v>23</v>
+      </c>
+      <c r="B24" s="50">
+        <v>0.12999999523162842</v>
+      </c>
+      <c r="C24" s="50">
+        <v>100</v>
+      </c>
+      <c r="D24" s="50">
+        <v>2</v>
+      </c>
+      <c r="E24" s="50">
+        <v>2</v>
+      </c>
+      <c r="F24" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="49">
+        <v>24</v>
+      </c>
+      <c r="B25" s="49">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="C25" s="49">
+        <v>100</v>
+      </c>
+      <c r="D25" s="49">
+        <v>2</v>
+      </c>
+      <c r="E25" s="49">
+        <v>0.22499999403953552</v>
+      </c>
+      <c r="F25" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="G25" s="49">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Change the method of value calculation
Change the method of value calculation
</commit_message>
<xml_diff>
--- a/Assets/testResult.xlsx
+++ b/Assets/testResult.xlsx
@@ -106,16 +106,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="0">
-        <v>0.20033268630504608</v>
+        <v>0.15000000596046448</v>
       </c>
       <c r="C2" s="0">
-        <v>129.7318115234375</v>
+        <v>110</v>
       </c>
       <c r="D2" s="0">
-        <v>0.67897719144821167</v>
+        <v>0.60000002384185791</v>
       </c>
       <c r="E2" s="0">
-        <v>1.2933487892150879</v>
+        <v>1.1999998092651367</v>
       </c>
       <c r="F2" s="0">
         <v>1</v>
@@ -126,16 +126,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="0">
-        <v>0.12692026793956757</v>
+        <v>0.20000001788139343</v>
       </c>
       <c r="C3" s="0">
-        <v>142.99090576171875</v>
+        <v>80</v>
       </c>
       <c r="D3" s="0">
-        <v>0.72748851776123047</v>
+        <v>0.70000004768371582</v>
       </c>
       <c r="E3" s="0">
-        <v>1.316786527633667</v>
+        <v>1.3499996662139893</v>
       </c>
       <c r="F3" s="0">
         <v>1</v>

</xml_diff>